<commit_message>
create agency boundaries with tigris
</commit_message>
<xml_diff>
--- a/follow_up_requests/trpd-wirth-home-locations/theodore_wirth_visitor_home_locations.xlsx
+++ b/follow_up_requests/trpd-wirth-home-locations/theodore_wirth_visitor_home_locations.xlsx
@@ -585,10 +585,10 @@
         <v>18</v>
       </c>
       <c r="B8" t="n">
-        <v>31796</v>
+        <v>31759</v>
       </c>
       <c r="C8" t="n">
-        <v>5.04407208573999</v>
+        <v>5.03811416273365</v>
       </c>
     </row>
     <row r="9">
@@ -596,10 +596,10 @@
         <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>8725</v>
+        <v>8716</v>
       </c>
       <c r="C9" t="n">
-        <v>1.38409928959878</v>
+        <v>1.38276494775071</v>
       </c>
     </row>
     <row r="10">
@@ -607,10 +607,10 @@
         <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>9534</v>
+        <v>9522</v>
       </c>
       <c r="C10" t="n">
-        <v>1.51243772524639</v>
+        <v>1.51062703476646</v>
       </c>
     </row>
     <row r="11">
@@ -618,10 +618,10 @@
         <v>21</v>
       </c>
       <c r="B11" t="n">
-        <v>9288</v>
+        <v>9285</v>
       </c>
       <c r="C11" t="n">
-        <v>1.47337232384573</v>
+        <v>1.47292319366238</v>
       </c>
     </row>
     <row r="12">
@@ -629,10 +629,10 @@
         <v>22</v>
       </c>
       <c r="B12" t="n">
-        <v>229715</v>
+        <v>229892</v>
       </c>
       <c r="C12" t="n">
-        <v>36.4415384241652</v>
+        <v>36.4696515855179</v>
       </c>
     </row>
     <row r="13">
@@ -640,10 +640,10 @@
         <v>23</v>
       </c>
       <c r="B13" t="n">
-        <v>19097</v>
+        <v>21216</v>
       </c>
       <c r="C13" t="n">
-        <v>3.02949675684237</v>
+        <v>3.36567549861431</v>
       </c>
     </row>
     <row r="14">
@@ -654,7 +654,7 @@
         <v>6702</v>
       </c>
       <c r="C14" t="n">
-        <v>1.06318697620617</v>
+        <v>1.06321126436847</v>
       </c>
     </row>
     <row r="15">
@@ -662,10 +662,10 @@
         <v>25</v>
       </c>
       <c r="B15" t="n">
-        <v>27619</v>
+        <v>27535</v>
       </c>
       <c r="C15" t="n">
-        <v>4.38143364076663</v>
+        <v>4.36809854758978</v>
       </c>
     </row>
     <row r="16">
@@ -673,10 +673,10 @@
         <v>26</v>
       </c>
       <c r="B16" t="n">
-        <v>254712</v>
+        <v>252567</v>
       </c>
       <c r="C16" t="n">
-        <v>40.4069979500081</v>
+        <v>40.0667248278992</v>
       </c>
     </row>
     <row r="17">
@@ -684,10 +684,10 @@
         <v>27</v>
       </c>
       <c r="B17" t="n">
-        <v>5972</v>
+        <v>5979</v>
       </c>
       <c r="C17" t="n">
-        <v>0.947409108996808</v>
+        <v>0.94846521487083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>